<commit_message>
Finished labeling the data
</commit_message>
<xml_diff>
--- a/venv/assets/postsArabic.xlsx
+++ b/venv/assets/postsArabic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ask-Banky-Classifier\venv\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56633E6-2127-435F-AAC2-BA304D2E9994}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97C71C4-47FB-4590-9A49-F4E2A338A112}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="1608" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="postsArabic" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="380">
   <si>
     <t>يوم الخميس اللي فات البنك المركزي خفض الفائدة 0.5% ↙️ وبالتالي البنوك بدأت تنفيذ القرار وتخفيض الفائدة على المنتجات البنكية 🏛 واللي منها الشهادات 📃\n\nلو بتدور على أسعار الفوائد على الشهادات المتغيرة، هتلاقيهم في تقرير النهارده في 21 بنك، واللي من خلاله هتقارن وتوصل لأفضل اختيار😎\n📎https://bankygate.com/15099</t>
   </si>
@@ -2010,8 +2010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C142" workbookViewId="0">
-      <selection activeCell="F145" sqref="F145"/>
+    <sheetView tabSelected="1" topLeftCell="C190" workbookViewId="0">
+      <selection activeCell="E195" sqref="E195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45.3984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4129,6 +4129,9 @@
       <c r="C151" t="s">
         <v>278</v>
       </c>
+      <c r="D151" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152">
@@ -4140,6 +4143,9 @@
       <c r="C152" t="s">
         <v>280</v>
       </c>
+      <c r="D152" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153">
@@ -4151,6 +4157,9 @@
       <c r="C153" t="s">
         <v>159</v>
       </c>
+      <c r="D153" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154">
@@ -4162,6 +4171,9 @@
       <c r="C154" t="s">
         <v>283</v>
       </c>
+      <c r="D154" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155">
@@ -4173,6 +4185,9 @@
       <c r="C155" t="s">
         <v>1</v>
       </c>
+      <c r="D155" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156">
@@ -4184,6 +4199,9 @@
       <c r="C156" t="s">
         <v>286</v>
       </c>
+      <c r="D156" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157">
@@ -4195,6 +4213,9 @@
       <c r="C157" t="s">
         <v>288</v>
       </c>
+      <c r="D157" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158">
@@ -4206,6 +4227,9 @@
       <c r="C158" t="s">
         <v>290</v>
       </c>
+      <c r="D158" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159">
@@ -4217,6 +4241,9 @@
       <c r="C159" t="s">
         <v>38</v>
       </c>
+      <c r="D159" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160">
@@ -4228,8 +4255,11 @@
       <c r="C160" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D160" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>161</v>
       </c>
@@ -4239,8 +4269,11 @@
       <c r="C161" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D161" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>162</v>
       </c>
@@ -4250,8 +4283,11 @@
       <c r="C162" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D162" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>163</v>
       </c>
@@ -4261,8 +4297,11 @@
       <c r="C163" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D163" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>164</v>
       </c>
@@ -4272,8 +4311,11 @@
       <c r="C164" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D164" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>165</v>
       </c>
@@ -4283,8 +4325,11 @@
       <c r="C165" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D165" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>166</v>
       </c>
@@ -4294,8 +4339,11 @@
       <c r="C166" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D166" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>167</v>
       </c>
@@ -4305,8 +4353,11 @@
       <c r="C167" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D167" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>168</v>
       </c>
@@ -4316,8 +4367,11 @@
       <c r="C168" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D168" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>169</v>
       </c>
@@ -4327,8 +4381,11 @@
       <c r="C169" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D169" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>170</v>
       </c>
@@ -4338,8 +4395,11 @@
       <c r="C170" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D170" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>171</v>
       </c>
@@ -4349,8 +4409,11 @@
       <c r="C171" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D171" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>172</v>
       </c>
@@ -4360,8 +4423,11 @@
       <c r="C172" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D172" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>173</v>
       </c>
@@ -4371,8 +4437,11 @@
       <c r="C173" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D173" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>174</v>
       </c>
@@ -4382,8 +4451,11 @@
       <c r="C174" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D174" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>175</v>
       </c>
@@ -4393,8 +4465,11 @@
       <c r="C175" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D175" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>176</v>
       </c>
@@ -4404,8 +4479,11 @@
       <c r="C176" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D176" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>177</v>
       </c>
@@ -4415,8 +4493,11 @@
       <c r="C177" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D177" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>178</v>
       </c>
@@ -4426,8 +4507,11 @@
       <c r="C178" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D178" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>179</v>
       </c>
@@ -4437,8 +4521,11 @@
       <c r="C179" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D179" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>180</v>
       </c>
@@ -4448,8 +4535,11 @@
       <c r="C180" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D180" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>181</v>
       </c>
@@ -4459,8 +4549,11 @@
       <c r="C181" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D181" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>182</v>
       </c>
@@ -4470,8 +4563,11 @@
       <c r="C182" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D182" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>183</v>
       </c>
@@ -4481,8 +4577,11 @@
       <c r="C183" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D183" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>184</v>
       </c>
@@ -4492,8 +4591,11 @@
       <c r="C184" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D184" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>185</v>
       </c>
@@ -4503,8 +4605,11 @@
       <c r="C185" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D185" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>186</v>
       </c>
@@ -4514,8 +4619,11 @@
       <c r="C186" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D186" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>187</v>
       </c>
@@ -4525,8 +4633,11 @@
       <c r="C187" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D187" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>188</v>
       </c>
@@ -4536,8 +4647,11 @@
       <c r="C188" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D188" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>189</v>
       </c>
@@ -4547,8 +4661,11 @@
       <c r="C189" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D189" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>190</v>
       </c>
@@ -4558,8 +4675,11 @@
       <c r="C190" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D190" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>191</v>
       </c>
@@ -4569,8 +4689,11 @@
       <c r="C191" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D191" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>192</v>
       </c>
@@ -4580,8 +4703,11 @@
       <c r="C192" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D192" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>193</v>
       </c>
@@ -4591,8 +4717,11 @@
       <c r="C193" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D193" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>194</v>
       </c>
@@ -4602,8 +4731,11 @@
       <c r="C194" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D194" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>195</v>
       </c>
@@ -4613,8 +4745,11 @@
       <c r="C195" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D195" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>196</v>
       </c>
@@ -4624,8 +4759,11 @@
       <c r="C196" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D196" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>197</v>
       </c>
@@ -4635,8 +4773,11 @@
       <c r="C197" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D197" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>198</v>
       </c>
@@ -4646,8 +4787,11 @@
       <c r="C198" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D198" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>199</v>
       </c>
@@ -4657,8 +4801,11 @@
       <c r="C199" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D199" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>200</v>
       </c>
@@ -4667,6 +4814,9 @@
       </c>
       <c r="C200" t="s">
         <v>369</v>
+      </c>
+      <c r="D200" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>